<commit_message>
My profile test added
</commit_message>
<xml_diff>
--- a/IdeaProjects/Promytheus/promy.xlsx
+++ b/IdeaProjects/Promytheus/promy.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="7755" windowWidth="20115" xWindow="240" yWindow="30"/>
+    <workbookView activeTab="2" windowHeight="7755" windowWidth="20115" xWindow="240" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="personal" r:id="rId1" sheetId="1"/>
     <sheet name="login" r:id="rId2" sheetId="2"/>
     <sheet name="users" r:id="rId3" sheetId="3"/>
+    <sheet name="emails" r:id="rId4" sheetId="4"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" name="LOCAL_MYSQL_DATE_FORMAT"><![CDATA[REPT(LOCAL_YEAR_FORMAT,4)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_MONTH_FORMAT,2)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_DAY_FORMAT,2)&" "&REPT(LOCAL_HOUR_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_MINUTE_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_SECOND_FORMAT,2)]]></definedName>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
   <si>
     <t>id</t>
   </si>
@@ -187,88 +188,73 @@
     <t>Password</t>
   </si>
   <si>
-    <t>hiwiwo@wmail.club</t>
-  </si>
-  <si>
-    <t>ntihswG0ws</t>
-  </si>
-  <si>
-    <t>kekodizy@nada.ltd</t>
-  </si>
-  <si>
-    <t>BBE4ofSo3y</t>
-  </si>
-  <si>
-    <t>debedede@cmail.club</t>
-  </si>
-  <si>
-    <t>tXGpyn9lUJ</t>
-  </si>
-  <si>
-    <t>hames@cars2.club</t>
-  </si>
-  <si>
-    <t>Wqbq5gjhyk</t>
-  </si>
-  <si>
-    <t>vily@cars2.club</t>
-  </si>
-  <si>
-    <t>59CPLmiavS</t>
-  </si>
-  <si>
-    <t>fyzixowo@banit.me</t>
-  </si>
-  <si>
-    <t>AuLWEhaGIG</t>
-  </si>
-  <si>
-    <t>lyxoq@duck2.club</t>
-  </si>
-  <si>
-    <t>IG9VzSh4PK</t>
-  </si>
-  <si>
-    <t>qipepy@banit.club</t>
-  </si>
-  <si>
-    <t>P9DdXNPmeW</t>
-  </si>
-  <si>
-    <t>patica@nada.ltd</t>
-  </si>
-  <si>
-    <t>yl61GQdRgS</t>
-  </si>
-  <si>
-    <t>cohoryxa@cmail.club</t>
-  </si>
-  <si>
-    <t>ILVHiWjnKs</t>
-  </si>
-  <si>
-    <t>xydyt@wmail.club</t>
-  </si>
-  <si>
-    <t>iRL4BwD2GM</t>
-  </si>
-  <si>
-    <t>nudu@banit.club</t>
-  </si>
-  <si>
-    <t>SuHjjg0Wae</t>
-  </si>
-  <si>
-    <t>pijyhij@banit.club</t>
-  </si>
-  <si>
-    <t>DhA4lX63hQ</t>
-  </si>
-  <si>
-    <t>gupo@banit.club</t>
-  </si>
-  <si>
-    <t>OK6vZCb6iv</t>
+    <t>invalid emails</t>
+  </si>
+  <si>
+    <t>plainaddress</t>
+  </si>
+  <si>
+    <t>#@%^%#$@#$@#.com</t>
+  </si>
+  <si>
+    <t>@domain.com</t>
+  </si>
+  <si>
+    <t>Joe Smith &lt;email@domain.com&gt;</t>
+  </si>
+  <si>
+    <t>email.domain.com</t>
+  </si>
+  <si>
+    <t>email@domain@domain.com</t>
+  </si>
+  <si>
+    <t>.email@domain.com</t>
+  </si>
+  <si>
+    <t>email.@domain.com</t>
+  </si>
+  <si>
+    <t>email..email@domain.com</t>
+  </si>
+  <si>
+    <t>あいうえお@domain.com</t>
+  </si>
+  <si>
+    <t>email@domain.com (Joe Smith)</t>
+  </si>
+  <si>
+    <t>email@domain</t>
+  </si>
+  <si>
+    <t>email@-domain.com</t>
+  </si>
+  <si>
+    <t>email@domain.web</t>
+  </si>
+  <si>
+    <t>email@111.222.333.44444</t>
+  </si>
+  <si>
+    <t>email@domain..com</t>
+  </si>
+  <si>
+    <t>jypudiry@amail.club</t>
+  </si>
+  <si>
+    <t>fEpkeCRVzY</t>
+  </si>
+  <si>
+    <t>dybo@banit.me</t>
+  </si>
+  <si>
+    <t>cqqCMyVmsi</t>
+  </si>
+  <si>
+    <t>buguma@duck2.club</t>
+  </si>
+  <si>
+    <t>tx5clQNdOu</t>
   </si>
 </sst>
 </file>
@@ -278,7 +264,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +293,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -329,7 +321,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
@@ -352,6 +344,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -929,7 +922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -1003,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1024,117 +1017,136 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
         <v>77</v>
-      </c>
-      <c r="B16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.42578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row ht="16.5" r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row ht="16.5" r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row ht="16.5" r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row ht="16.5" r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row ht="16.5" r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row ht="16.5" r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row ht="16.5" r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row ht="16.5" r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row ht="16.5" r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row ht="16.5" r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row ht="16.5" r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row ht="16.5" r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row ht="16.5" r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row ht="16.5" r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row ht="16.5" r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A9"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId2" verticalDpi="4294967293"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
data provider random added
</commit_message>
<xml_diff>
--- a/IdeaProjects/Promytheus/promy.xlsx
+++ b/IdeaProjects/Promytheus/promy.xlsx
@@ -4,24 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="7755" windowWidth="20115" xWindow="240" yWindow="30"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="personal" r:id="rId1" sheetId="1"/>
-    <sheet name="login" r:id="rId2" sheetId="2"/>
-    <sheet name="users" r:id="rId3" sheetId="3"/>
-    <sheet name="emails" r:id="rId4" sheetId="4"/>
+    <sheet name="personal" sheetId="1" r:id="rId1"/>
+    <sheet name="login" sheetId="2" r:id="rId2"/>
+    <sheet name="users" sheetId="3" r:id="rId3"/>
+    <sheet name="emails" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" name="LOCAL_MYSQL_DATE_FORMAT"><![CDATA[REPT(LOCAL_YEAR_FORMAT,4)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_MONTH_FORMAT,2)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_DAY_FORMAT,2)&" "&REPT(LOCAL_HOUR_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_MINUTE_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_SECOND_FORMAT,2)]]></definedName>
-    <definedName hidden="1" name="LOCAL_SECOND_FORMAT">" "</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_SECOND_FORMAT" hidden="1">" "</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
   <si>
     <t>id</t>
   </si>
@@ -237,36 +237,6 @@
   </si>
   <si>
     <t>email@domain..com</t>
-  </si>
-  <si>
-    <t>jypudiry@amail.club</t>
-  </si>
-  <si>
-    <t>fEpkeCRVzY</t>
-  </si>
-  <si>
-    <t>dybo@banit.me</t>
-  </si>
-  <si>
-    <t>cqqCMyVmsi</t>
-  </si>
-  <si>
-    <t>buguma@duck2.club</t>
-  </si>
-  <si>
-    <t>tx5clQNdOu</t>
-  </si>
-  <si>
-    <t>cicywuj@wmail.club</t>
-  </si>
-  <si>
-    <t>JYyDQslusd</t>
-  </si>
-  <si>
-    <t>givimesa@banit.me</t>
-  </si>
-  <si>
-    <t>WG4wankI2w</t>
   </si>
 </sst>
 </file>
@@ -330,37 +300,37 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -386,10 +356,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
-    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
-      <tableStyleElement dxfId="1" type="wholeTable"/>
-      <tableStyleElement dxfId="0" type="headerRow"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -405,10 +375,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -566,7 +536,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -575,13 +545,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -591,7 +561,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -600,7 +570,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -609,7 +579,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -619,12 +589,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -655,7 +625,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -674,7 +644,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -686,32 +656,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0" zoomScaleNormal="100">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="2.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="14.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="19.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="27.5703125" collapsed="true"/>
-    <col min="9" max="9" style="2" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="14.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="11.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="9.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="27.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="19.5703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="11.5703125" collapsed="true"/>
-    <col min="16" max="17" bestFit="true" customWidth="true" style="2" width="9.28515625" collapsed="true"/>
-    <col min="18" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="2.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="2" collapsed="1"/>
+    <col min="10" max="10" width="14.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="27.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="9.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
@@ -925,13 +895,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="4294967293"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -940,7 +910,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -995,25 +965,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A6"/>
-    <hyperlink r:id="rId2" ref="A5"/>
-    <hyperlink r:id="rId3" ref="A4"/>
-    <hyperlink r:id="rId4" ref="A7"/>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="A5" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId4"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1024,56 +994,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1082,7 +1009,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1090,37 +1017,37 @@
         <v>55</v>
       </c>
     </row>
-    <row ht="16.5" r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row ht="16.5" r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row ht="16.5" r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row ht="16.5" r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row ht="16.5" r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row ht="16.5" r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row ht="16.5" r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>62</v>
       </c>
@@ -1130,51 +1057,51 @@
         <v>63</v>
       </c>
     </row>
-    <row ht="16.5" r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row ht="16.5" r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row ht="16.5" r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row ht="16.5" r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row ht="16.5" r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row ht="16.5" r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row ht="16.5" r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row ht="16.5" r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A9"/>
+    <hyperlink ref="A9" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId2" verticalDpi="4294967293"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>